<commit_message>
add  certificate and redy for server migrate
</commit_message>
<xml_diff>
--- a/database/plantilla/PlantillaDatosMaestros.xlsx
+++ b/database/plantilla/PlantillaDatosMaestros.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t>Primer Nombre</t>
   </si>
@@ -333,12 +333,6 @@
     <t>matematica</t>
   </si>
   <si>
-    <t>materias</t>
-  </si>
-  <si>
-    <t>fisica</t>
-  </si>
-  <si>
     <t>historia</t>
   </si>
   <si>
@@ -372,15 +366,6 @@
     <t>grado</t>
   </si>
   <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t>3A</t>
-  </si>
-  <si>
     <t>situacion alumno</t>
   </si>
   <si>
@@ -435,12 +420,6 @@
     <t>otro</t>
   </si>
   <si>
-    <t>area estudio</t>
-  </si>
-  <si>
-    <t>sociales</t>
-  </si>
-  <si>
     <t>fisica I</t>
   </si>
   <si>
@@ -460,13 +439,82 @@
   </si>
   <si>
     <t>Estado Civil</t>
+  </si>
+  <si>
+    <t>Colegios Amigos del Turismo</t>
+  </si>
+  <si>
+    <t>Educación Continua</t>
+  </si>
+  <si>
+    <t>Consultoría</t>
+  </si>
+  <si>
+    <t>Turismo Académico</t>
+  </si>
+  <si>
+    <t>Curso Internación Opción de Grado</t>
+  </si>
+  <si>
+    <t>Programa</t>
+  </si>
+  <si>
+    <t>Cursos/Materias</t>
+  </si>
+  <si>
+    <t>Bilingüismo Social</t>
+  </si>
+  <si>
+    <t>Dis. e Innov. Productos Turísticos</t>
+  </si>
+  <si>
+    <t>Fortalecimiento Empresarial</t>
+  </si>
+  <si>
+    <t>Inmersión Ingles</t>
+  </si>
+  <si>
+    <t>Turismo Científico</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>superior</t>
+  </si>
+  <si>
+    <t>4º Grado</t>
+  </si>
+  <si>
+    <t>Colegio 1A</t>
+  </si>
+  <si>
+    <t>Colegio 1B</t>
+  </si>
+  <si>
+    <t>Colegio 1C</t>
+  </si>
+  <si>
+    <t>Ingles A1</t>
+  </si>
+  <si>
+    <t>Ingles A2</t>
+  </si>
+  <si>
+    <t>Ingles A3</t>
+  </si>
+  <si>
+    <t>Programa/Areas Estudio</t>
+  </si>
+  <si>
+    <t>Asignatura/Tema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,19 +542,66 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -515,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -524,11 +619,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -542,10 +675,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -561,16 +694,76 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="G1:H4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="I1:J6" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="materias"/>
-    <tableColumn id="2" name="area estudio"/>
+    <tableColumn id="1" name="Cursos/Materias"/>
+    <tableColumn id="2" name="Programa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:S444" totalsRowShown="0" headerRowDxfId="7">
+  <tableColumns count="19">
+    <tableColumn id="16" name="NRO"/>
+    <tableColumn id="1" name="documento"/>
+    <tableColumn id="2" name="Primer Nombre"/>
+    <tableColumn id="3" name="Segundo Nombre"/>
+    <tableColumn id="4" name="Primer Apellido"/>
+    <tableColumn id="5" name="Segundo Apellido"/>
+    <tableColumn id="6" name="sexo" dataDxfId="6"/>
+    <tableColumn id="7" name="Fecha Nacimiento"/>
+    <tableColumn id="8" name="Nacionalidad"/>
+    <tableColumn id="9" name="Lugar de Nacimiento"/>
+    <tableColumn id="10" name="departamento"/>
+    <tableColumn id="11" name="ciudad"/>
+    <tableColumn id="12" name="direccion"/>
+    <tableColumn id="13" name="telefono"/>
+    <tableColumn id="14" name="telefono2"/>
+    <tableColumn id="15" name="email"/>
+    <tableColumn id="17" name="situacion alumno"/>
+    <tableColumn id="18" name="grado"/>
+    <tableColumn id="19" name="grupo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla145" displayName="Tabla145" ref="A1:Y444" totalsRowShown="0" headerRowDxfId="5">
+  <tableColumns count="25">
+    <tableColumn id="16" name="NRO"/>
+    <tableColumn id="1" name="documento"/>
+    <tableColumn id="2" name="Primer Nombre"/>
+    <tableColumn id="3" name="Segundo Nombre"/>
+    <tableColumn id="4" name="Primer Apellido"/>
+    <tableColumn id="5" name="Segundo Apellido"/>
+    <tableColumn id="6" name="sexo" dataDxfId="4"/>
+    <tableColumn id="7" name="Fecha Nacimiento"/>
+    <tableColumn id="26" name="Estado Civil"/>
+    <tableColumn id="8" name="Nacionalidad"/>
+    <tableColumn id="9" name="Lugar de Nacimiento"/>
+    <tableColumn id="10" name="departamento"/>
+    <tableColumn id="11" name="ciudad"/>
+    <tableColumn id="12" name="direccion"/>
+    <tableColumn id="13" name="telefono"/>
+    <tableColumn id="14" name="telefono2"/>
+    <tableColumn id="15" name="email"/>
+    <tableColumn id="17" name="alumno 1"/>
+    <tableColumn id="22" name="parentesco 1"/>
+    <tableColumn id="18" name="alumno 2"/>
+    <tableColumn id="23" name="parntesco 2"/>
+    <tableColumn id="19" name="alumno 3"/>
+    <tableColumn id="24" name="parentesco 3"/>
+    <tableColumn id="20" name="alumno 4"/>
+    <tableColumn id="25" name="parentesco 4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla14" displayName="Tabla14" ref="A1:X444" totalsRowShown="0" headerRowDxfId="3">
   <tableColumns count="24">
     <tableColumn id="16" name="NRO"/>
@@ -603,7 +796,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla57" displayName="Tabla57" ref="L1:M4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla57" displayName="Tabla57" ref="N1:O5" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="grados"/>
     <tableColumn id="2" name="nivel"/>
@@ -613,7 +806,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="J1:J4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="L1:L6" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="nivel"/>
   </tableColumns>
@@ -622,7 +815,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla5710" displayName="Tabla5710" ref="O1:P4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla5710" displayName="Tabla5710" ref="Q1:R4" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="grupo"/>
     <tableColumn id="2" name="grado"/>
@@ -660,60 +853,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:S444" totalsRowShown="0" headerRowDxfId="4">
-  <tableColumns count="19">
-    <tableColumn id="16" name="NRO"/>
-    <tableColumn id="1" name="documento"/>
-    <tableColumn id="2" name="Primer Nombre"/>
-    <tableColumn id="3" name="Segundo Nombre"/>
-    <tableColumn id="4" name="Primer Apellido"/>
-    <tableColumn id="5" name="Segundo Apellido"/>
-    <tableColumn id="6" name="sexo" dataDxfId="5"/>
-    <tableColumn id="7" name="Fecha Nacimiento"/>
-    <tableColumn id="8" name="Nacionalidad"/>
-    <tableColumn id="9" name="Lugar de Nacimiento"/>
-    <tableColumn id="10" name="departamento"/>
-    <tableColumn id="11" name="ciudad"/>
-    <tableColumn id="12" name="direccion"/>
-    <tableColumn id="13" name="telefono"/>
-    <tableColumn id="14" name="telefono2"/>
-    <tableColumn id="15" name="email"/>
-    <tableColumn id="17" name="situacion alumno"/>
-    <tableColumn id="18" name="grado"/>
-    <tableColumn id="19" name="grupo"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="G1:G6" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="G1:G6"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Programa/Areas Estudio"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla145" displayName="Tabla145" ref="A1:Y444" totalsRowShown="0" headerRowDxfId="1">
-  <tableColumns count="25">
-    <tableColumn id="16" name="NRO"/>
-    <tableColumn id="1" name="documento"/>
-    <tableColumn id="2" name="Primer Nombre"/>
-    <tableColumn id="3" name="Segundo Nombre"/>
-    <tableColumn id="4" name="Primer Apellido"/>
-    <tableColumn id="5" name="Segundo Apellido"/>
-    <tableColumn id="6" name="sexo" dataDxfId="0"/>
-    <tableColumn id="7" name="Fecha Nacimiento"/>
-    <tableColumn id="26" name="Estado Civil"/>
-    <tableColumn id="8" name="Nacionalidad"/>
-    <tableColumn id="9" name="Lugar de Nacimiento"/>
-    <tableColumn id="10" name="departamento"/>
-    <tableColumn id="11" name="ciudad"/>
-    <tableColumn id="12" name="direccion"/>
-    <tableColumn id="13" name="telefono"/>
-    <tableColumn id="14" name="telefono2"/>
-    <tableColumn id="15" name="email"/>
-    <tableColumn id="17" name="alumno 1"/>
-    <tableColumn id="22" name="parentesco 1"/>
-    <tableColumn id="18" name="alumno 2"/>
-    <tableColumn id="23" name="parntesco 2"/>
-    <tableColumn id="19" name="alumno 3"/>
-    <tableColumn id="24" name="parentesco 3"/>
-    <tableColumn id="20" name="alumno 4"/>
-    <tableColumn id="25" name="parentesco 4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla57108" displayName="Tabla57108" ref="T1:U4" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Asignatura/Tema"/>
+    <tableColumn id="2" name="grado"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -985,10 +1138,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,171 +1152,245 @@
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="4.140625" customWidth="1"/>
-    <col min="7" max="8" width="27" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="3.85546875" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="3" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" t="s">
+        <v>94</v>
+      </c>
+      <c r="U2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" t="s">
+        <v>96</v>
+      </c>
+      <c r="U4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
-      <formula1>$J$2:$J$25</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O1048576">
+      <formula1>$L$2:$L$25</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576">
-      <formula1>$L$2:$L$65</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1:R1048576 U1:U4">
+      <formula1>$N$2:$N$65</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576">
+      <formula1>$G$2:$G$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="7">
+  <tableParts count="9">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -1171,6 +1398,8 @@
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1182,8 +1411,8 @@
   </sheetPr>
   <dimension ref="A1:S444"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D444" sqref="D444"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,13 +1485,13 @@
         <v>13</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1315,13 +1544,13 @@
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -3560,13 +3789,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>datos!$L$2:$L$91</xm:f>
+            <xm:f>datos!$N$2:$N$91</xm:f>
           </x14:formula1>
           <xm:sqref>R2:R444</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>datos!$O$2:$O$277</xm:f>
+            <xm:f>datos!$Q$2:$Q$277</xm:f>
           </x14:formula1>
           <xm:sqref>S2:S444</xm:sqref>
         </x14:dataValidation>
@@ -3590,7 +3819,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3639,7 +3868,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
@@ -3666,28 +3895,28 @@
         <v>13</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -3716,7 +3945,7 @@
         <v>40766</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
         <v>31</v>
@@ -3746,7 +3975,7 @@
         <v>13479149</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3817,7 +4046,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,7 +4095,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
@@ -3940,7 +4169,7 @@
         <v>40401</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -3967,13 +4196,13 @@
         <v>22</v>
       </c>
       <c r="R2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S2" t="s">
         <v>39</v>
       </c>
       <c r="T2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4002,7 +4231,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>datos!$G$2:$G$190</xm:f>
+            <xm:f>datos!$I$2:$I$190</xm:f>
           </x14:formula1>
           <xm:sqref>R2:X1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>